<commit_message>
move to new server
</commit_message>
<xml_diff>
--- a/areas/1/160.xlsx
+++ b/areas/1/160.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1\zuy\areas\1\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1852D9F-0EE1-44E0-B99B-86E40833B4DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +30,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -340,18 +334,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -364,7 +358,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>